<commit_message>
Update economic data 2025-06-30
</commit_message>
<xml_diff>
--- a/data/長期系列_CI指数_DI指数_DI景気指標.xlsx
+++ b/data/長期系列_CI指数_DI指数_DI景気指標.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\CI\０１／CI\０１／速報\★R7(2025)★\令和7年4月分\g研究所ホームページ掲載宛送付ファイル\jp\stat\di\di\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\CI\０１／CI\０２／速報からの改訂\★R7(2025)★\令和7年4月改訂\g研究所ホームページ掲載宛送付ファイル\jp\stat\di\di\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B655297-534E-4348-B742-81684AA2DEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CB927DC-6816-4077-B794-3460D84D30C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
   </bookViews>
   <sheets>
     <sheet name="指数 Indexes" sheetId="1" r:id="rId1"/>
@@ -2805,11 +2805,11 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.109375" customWidth="1"/>
-    <col min="4" max="15" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.08984375" customWidth="1"/>
+    <col min="4" max="15" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="36" x14ac:dyDescent="0.2">
@@ -2944,7 +2944,7 @@
       </c>
       <c r="P3" s="5"/>
     </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" ht="32.4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" s="1" customFormat="1" ht="33" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>20</v>
       </c>
@@ -2992,7 +2992,7 @@
       </c>
       <c r="P4" s="5"/>
     </row>
-    <row r="5" spans="1:16" s="1" customFormat="1" ht="22.2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -27823,7 +27823,7 @@
         <v>115.8</v>
       </c>
       <c r="F549" s="4">
-        <v>111.2</v>
+        <v>111</v>
       </c>
       <c r="G549" s="4">
         <v>109.9</v>
@@ -27832,7 +27832,7 @@
         <v>114.2</v>
       </c>
       <c r="I549" s="4">
-        <v>109.2</v>
+        <v>109</v>
       </c>
       <c r="J549" s="4">
         <v>54.5</v>
@@ -27864,40 +27864,40 @@
         <v>4</v>
       </c>
       <c r="D550" s="4">
-        <v>103.4</v>
+        <v>104.2</v>
       </c>
       <c r="E550" s="4">
-        <v>115.5</v>
+        <v>116</v>
       </c>
       <c r="F550" s="4">
         <v>112.5</v>
       </c>
       <c r="G550" s="4">
-        <v>102.6</v>
+        <v>103.5</v>
       </c>
       <c r="H550" s="4">
-        <v>113.9</v>
+        <v>114.4</v>
       </c>
       <c r="I550" s="4">
-        <v>110.4</v>
+        <v>110.5</v>
       </c>
       <c r="J550" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K550" s="4">
+        <v>38.9</v>
+      </c>
+      <c r="L550" s="4">
         <v>43.8</v>
       </c>
-      <c r="L550" s="4">
-        <v>50</v>
-      </c>
       <c r="M550" s="4">
-        <v>1217.2</v>
+        <v>1227.2</v>
       </c>
       <c r="N550" s="4">
-        <v>3278.8</v>
+        <v>3273.9</v>
       </c>
       <c r="O550" s="4">
-        <v>3213</v>
+        <v>3206.8</v>
       </c>
     </row>
     <row r="559" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update economic data 2025-08-11
</commit_message>
<xml_diff>
--- a/data/長期系列_CI指数_DI指数_DI景気指標.xlsx
+++ b/data/長期系列_CI指数_DI指数_DI景気指標.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\CI\０１／CI\０２／速報からの改訂\★R7(2025)★\令和7年5月改訂\g研究所ホームページ掲載宛送付ファイル\jp\stat\di\di\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\CI\０１／CI\０１／速報\★R7(2025)★\令和7年6月分\g研究所ホームページ掲載宛送付ファイル\jp\stat\di\di\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A93CDBB-8524-4975-83E4-B7E49952A5DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D2194F5-2FD2-46E2-B828-40FDE25D41A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
   </bookViews>
   <sheets>
     <sheet name="指数 Indexes" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="570">
   <si>
     <t>ＤＩ指数</t>
   </si>
@@ -2299,6 +2299,10 @@
   </si>
   <si>
     <t>2025000505</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2025000606</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -2800,7 +2804,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P560"/>
+  <dimension ref="A1:P561"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
@@ -2809,11 +2813,11 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.109375" customWidth="1"/>
-    <col min="4" max="15" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.08984375" customWidth="1"/>
+    <col min="4" max="15" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="36" x14ac:dyDescent="0.2">
@@ -2948,7 +2952,7 @@
       </c>
       <c r="P3" s="5"/>
     </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" ht="32.4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" s="1" customFormat="1" ht="33" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>20</v>
       </c>
@@ -2996,7 +3000,7 @@
       </c>
       <c r="P4" s="5"/>
     </row>
-    <row r="5" spans="1:16" s="1" customFormat="1" ht="22.2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -27951,13 +27955,60 @@
         <v>3206.8</v>
       </c>
     </row>
-    <row r="560" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D560" s="3"/>
-      <c r="E560" s="3"/>
-      <c r="F560" s="3"/>
-      <c r="G560" s="3"/>
-      <c r="H560" s="3"/>
-      <c r="I560" s="3"/>
+    <row r="552" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A552" s="13" t="s">
+        <v>569</v>
+      </c>
+      <c r="B552" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C552" s="2">
+        <v>6</v>
+      </c>
+      <c r="D552" s="4">
+        <v>106.1</v>
+      </c>
+      <c r="E552" s="4">
+        <v>116.8</v>
+      </c>
+      <c r="F552" s="4">
+        <v>112</v>
+      </c>
+      <c r="G552" s="4">
+        <v>105.8</v>
+      </c>
+      <c r="H552" s="4">
+        <v>115.5</v>
+      </c>
+      <c r="I552" s="4">
+        <v>110.5</v>
+      </c>
+      <c r="J552" s="4">
+        <v>44.4</v>
+      </c>
+      <c r="K552" s="4">
+        <v>50</v>
+      </c>
+      <c r="L552" s="4">
+        <v>50</v>
+      </c>
+      <c r="M552" s="4">
+        <v>1211.5999999999999</v>
+      </c>
+      <c r="N552" s="4">
+        <v>3262.8</v>
+      </c>
+      <c r="O552" s="4">
+        <v>3206.8</v>
+      </c>
+    </row>
+    <row r="561" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D561" s="3"/>
+      <c r="E561" s="3"/>
+      <c r="F561" s="3"/>
+      <c r="G561" s="3"/>
+      <c r="H561" s="3"/>
+      <c r="I561" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
Update economic data 2025-10-06
</commit_message>
<xml_diff>
--- a/data/長期系列_CI指数_DI指数_DI景気指標.xlsx
+++ b/data/長期系列_CI指数_DI指数_DI景気指標.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\CI\０１／CI\０１／速報\★R7(2025)★\令和7年7月分\g研究所ホームページ掲載宛送付ファイル\jp\stat\di\di\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\CI\０１／CI\０２／速報からの改訂\★R7(2025)★\令和7年7月改訂\g研究所ホームページ掲載宛送付ファイル\jp\stat\di\di\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB87A4AA-AA2E-42B0-85F5-431787411CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{28AA724F-435D-4330-91B6-CCB8EC512961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
@@ -27882,7 +27882,7 @@
         <v>115.8</v>
       </c>
       <c r="F550" s="4">
-        <v>112.9</v>
+        <v>112.8</v>
       </c>
       <c r="G550" s="4">
         <v>104</v>
@@ -27970,25 +27970,25 @@
         <v>6</v>
       </c>
       <c r="D552" s="4">
-        <v>105.1</v>
+        <v>105</v>
       </c>
       <c r="E552" s="4">
         <v>115.9</v>
       </c>
       <c r="F552" s="4">
-        <v>113.4</v>
+        <v>113.2</v>
       </c>
       <c r="G552" s="4">
-        <v>105.2</v>
+        <v>105.1</v>
       </c>
       <c r="H552" s="4">
         <v>114.2</v>
       </c>
       <c r="I552" s="4">
-        <v>111.5</v>
+        <v>111.3</v>
       </c>
       <c r="J552" s="4">
-        <v>36.4</v>
+        <v>31.8</v>
       </c>
       <c r="K552" s="4">
         <v>50</v>
@@ -27997,7 +27997,7 @@
         <v>66.7</v>
       </c>
       <c r="M552" s="4">
-        <v>1199.2</v>
+        <v>1194.5999999999999</v>
       </c>
       <c r="N552" s="4">
         <v>3195</v>
@@ -28017,40 +28017,40 @@
         <v>7</v>
       </c>
       <c r="D553" s="4">
-        <v>105.9</v>
+        <v>106.1</v>
       </c>
       <c r="E553" s="4">
-        <v>113.3</v>
+        <v>114.1</v>
       </c>
       <c r="F553" s="4">
-        <v>114.2</v>
+        <v>113.6</v>
       </c>
       <c r="G553" s="4">
-        <v>106.2</v>
+        <v>106.3</v>
       </c>
       <c r="H553" s="4">
-        <v>111.6</v>
+        <v>112.4</v>
       </c>
       <c r="I553" s="4">
-        <v>112.2</v>
+        <v>111.7</v>
       </c>
       <c r="J553" s="4">
-        <v>66.7</v>
+        <v>60</v>
       </c>
       <c r="K553" s="4">
-        <v>25</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="L553" s="4">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="M553" s="4">
-        <v>1215.9000000000001</v>
+        <v>1204.5999999999999</v>
       </c>
       <c r="N553" s="4">
-        <v>3170</v>
+        <v>3178.3</v>
       </c>
       <c r="O553" s="4">
-        <v>3299.3</v>
+        <v>3324.3</v>
       </c>
     </row>
     <row r="562" spans="4:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update economic data 2025-11-17
</commit_message>
<xml_diff>
--- a/data/長期系列_CI指数_DI指数_DI景気指標.xlsx
+++ b/data/長期系列_CI指数_DI指数_DI景気指標.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\CI\０１／CI\０２／速報からの改訂\★R7(2025)★\令和7年8月改訂\g研究所ホームページ掲載宛送付ファイル\jp\stat\di\di\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\CI\０１／CI\０１／速報\★R7(2025)★\令和7年9月分\g研究所ホームページ掲載宛送付ファイル\jp\stat\di\di\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A09BF87-86C0-40EF-98EB-E82691B9E483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{89A87688-D12B-4CB7-89CF-0CAA95527FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="573">
   <si>
     <t>ＤＩ指数</t>
   </si>
@@ -2311,6 +2311,10 @@
   </si>
   <si>
     <t>2025000808</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2025000909</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -2812,7 +2816,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P563"/>
+  <dimension ref="A1:P564"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
@@ -28104,13 +28108,60 @@
         <v>3311.8</v>
       </c>
     </row>
-    <row r="563" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D563" s="3"/>
-      <c r="E563" s="3"/>
-      <c r="F563" s="3"/>
-      <c r="G563" s="3"/>
-      <c r="H563" s="3"/>
-      <c r="I563" s="3"/>
+    <row r="555" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A555" s="13" t="s">
+        <v>572</v>
+      </c>
+      <c r="B555" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C555" s="2">
+        <v>9</v>
+      </c>
+      <c r="D555" s="4">
+        <v>108</v>
+      </c>
+      <c r="E555" s="4">
+        <v>114.6</v>
+      </c>
+      <c r="F555" s="4">
+        <v>113.2</v>
+      </c>
+      <c r="G555" s="4">
+        <v>108.2</v>
+      </c>
+      <c r="H555" s="4">
+        <v>113</v>
+      </c>
+      <c r="I555" s="4">
+        <v>111.2</v>
+      </c>
+      <c r="J555" s="4">
+        <v>77.8</v>
+      </c>
+      <c r="K555" s="4">
+        <v>25</v>
+      </c>
+      <c r="L555" s="4">
+        <v>25</v>
+      </c>
+      <c r="M555" s="4">
+        <v>1242.4000000000001</v>
+      </c>
+      <c r="N555" s="4">
+        <v>3103.3</v>
+      </c>
+      <c r="O555" s="4">
+        <v>3286.8</v>
+      </c>
+    </row>
+    <row r="564" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D564" s="3"/>
+      <c r="E564" s="3"/>
+      <c r="F564" s="3"/>
+      <c r="G564" s="3"/>
+      <c r="H564" s="3"/>
+      <c r="I564" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
Update economic data 2025-12-29
</commit_message>
<xml_diff>
--- a/data/長期系列_CI指数_DI指数_DI景気指標.xlsx
+++ b/data/長期系列_CI指数_DI指数_DI景気指標.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\CI\０１／CI\０１／速報\★R7(2025)★\令和7年10月分\g研究所ホームページ掲載宛送付ファイル\jp\stat\di\di\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\CI\０１／CI\０２／速報からの改訂\★R7(2025)★\令和7年10月改訂\g研究所ホームページ掲載宛送付ファイル\jp\stat\di\di\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9AAED845-7478-42C1-A648-FE366EEBCB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{91D86F4C-B40C-45B0-A9AF-48EEA40268E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
@@ -26,6 +26,9 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -5193,7 +5196,7 @@
         <v>90.8</v>
       </c>
       <c r="F67" s="4">
-        <v>85</v>
+        <v>84.9</v>
       </c>
       <c r="G67" s="4">
         <v>88.4</v>
@@ -5249,7 +5252,7 @@
         <v>93</v>
       </c>
       <c r="I68" s="4">
-        <v>84.9</v>
+        <v>84.8</v>
       </c>
       <c r="J68" s="4">
         <v>45.5</v>
@@ -5334,7 +5337,7 @@
         <v>91.4</v>
       </c>
       <c r="F70" s="4">
-        <v>86</v>
+        <v>85.9</v>
       </c>
       <c r="G70" s="4">
         <v>89.3</v>
@@ -5343,7 +5346,7 @@
         <v>94</v>
       </c>
       <c r="I70" s="4">
-        <v>86.2</v>
+        <v>86.1</v>
       </c>
       <c r="J70" s="4">
         <v>63.6</v>
@@ -5381,7 +5384,7 @@
         <v>91.3</v>
       </c>
       <c r="F71" s="4">
-        <v>86</v>
+        <v>85.9</v>
       </c>
       <c r="G71" s="4">
         <v>89.3</v>
@@ -5428,7 +5431,7 @@
         <v>90.6</v>
       </c>
       <c r="F72" s="4">
-        <v>86.4</v>
+        <v>86.3</v>
       </c>
       <c r="G72" s="4">
         <v>88.6</v>
@@ -5475,7 +5478,7 @@
         <v>91.6</v>
       </c>
       <c r="F73" s="4">
-        <v>87.5</v>
+        <v>87.4</v>
       </c>
       <c r="G73" s="4">
         <v>88.5</v>
@@ -5484,7 +5487,7 @@
         <v>94.3</v>
       </c>
       <c r="I73" s="4">
-        <v>87.6</v>
+        <v>87.5</v>
       </c>
       <c r="J73" s="4">
         <v>45.5</v>
@@ -5578,7 +5581,7 @@
         <v>93.7</v>
       </c>
       <c r="I75" s="4">
-        <v>87.3</v>
+        <v>87.2</v>
       </c>
       <c r="J75" s="4">
         <v>36.4</v>
@@ -5898,7 +5901,7 @@
         <v>90.1</v>
       </c>
       <c r="F82" s="4">
-        <v>85.6</v>
+        <v>85.5</v>
       </c>
       <c r="G82" s="4">
         <v>85.9</v>
@@ -5907,7 +5910,7 @@
         <v>92.8</v>
       </c>
       <c r="I82" s="4">
-        <v>86.4</v>
+        <v>86.3</v>
       </c>
       <c r="J82" s="4">
         <v>36.4</v>
@@ -6086,7 +6089,7 @@
         <v>88.5</v>
       </c>
       <c r="F86" s="4">
-        <v>85.5</v>
+        <v>85.4</v>
       </c>
       <c r="G86" s="4">
         <v>85</v>
@@ -6095,7 +6098,7 @@
         <v>91.1</v>
       </c>
       <c r="I86" s="4">
-        <v>86.2</v>
+        <v>86.1</v>
       </c>
       <c r="J86" s="4">
         <v>50</v>
@@ -6133,7 +6136,7 @@
         <v>90.1</v>
       </c>
       <c r="F87" s="4">
-        <v>85.8</v>
+        <v>85.7</v>
       </c>
       <c r="G87" s="4">
         <v>84.6</v>
@@ -6142,7 +6145,7 @@
         <v>92.7</v>
       </c>
       <c r="I87" s="4">
-        <v>87</v>
+        <v>86.9</v>
       </c>
       <c r="J87" s="4">
         <v>72.7</v>
@@ -6180,7 +6183,7 @@
         <v>89.5</v>
       </c>
       <c r="F88" s="4">
-        <v>85.8</v>
+        <v>85.7</v>
       </c>
       <c r="G88" s="4">
         <v>84</v>
@@ -6236,7 +6239,7 @@
         <v>91.3</v>
       </c>
       <c r="I89" s="4">
-        <v>86.2</v>
+        <v>86.1</v>
       </c>
       <c r="J89" s="4">
         <v>36.4</v>
@@ -6283,7 +6286,7 @@
         <v>92.3</v>
       </c>
       <c r="I90" s="4">
-        <v>86.3</v>
+        <v>86.2</v>
       </c>
       <c r="J90" s="4">
         <v>72.7</v>
@@ -6556,7 +6559,7 @@
         <v>93.3</v>
       </c>
       <c r="F96" s="4">
-        <v>86.2</v>
+        <v>86.1</v>
       </c>
       <c r="G96" s="4">
         <v>94.5</v>
@@ -6697,7 +6700,7 @@
         <v>96.3</v>
       </c>
       <c r="F99" s="4">
-        <v>88.4</v>
+        <v>88.3</v>
       </c>
       <c r="G99" s="4">
         <v>98.2</v>
@@ -6706,7 +6709,7 @@
         <v>99.2</v>
       </c>
       <c r="I99" s="4">
-        <v>89.6</v>
+        <v>89.5</v>
       </c>
       <c r="J99" s="4">
         <v>81.8</v>
@@ -6791,7 +6794,7 @@
         <v>98.5</v>
       </c>
       <c r="F101" s="4">
-        <v>89.3</v>
+        <v>89.2</v>
       </c>
       <c r="G101" s="4">
         <v>101.3</v>
@@ -6885,7 +6888,7 @@
         <v>100.3</v>
       </c>
       <c r="F103" s="4">
-        <v>90.7</v>
+        <v>90.6</v>
       </c>
       <c r="G103" s="4">
         <v>102.6</v>
@@ -6941,7 +6944,7 @@
         <v>105.6</v>
       </c>
       <c r="I104" s="4">
-        <v>93</v>
+        <v>92.9</v>
       </c>
       <c r="J104" s="4">
         <v>77.3</v>
@@ -6979,7 +6982,7 @@
         <v>101.3</v>
       </c>
       <c r="F105" s="4">
-        <v>92.6</v>
+        <v>92.5</v>
       </c>
       <c r="G105" s="4">
         <v>102.8</v>
@@ -7026,7 +7029,7 @@
         <v>103.4</v>
       </c>
       <c r="F106" s="4">
-        <v>93</v>
+        <v>92.9</v>
       </c>
       <c r="G106" s="4">
         <v>103.1</v>
@@ -7035,7 +7038,7 @@
         <v>106.4</v>
       </c>
       <c r="I106" s="4">
-        <v>94.7</v>
+        <v>94.6</v>
       </c>
       <c r="J106" s="4">
         <v>36.4</v>
@@ -7073,7 +7076,7 @@
         <v>102.8</v>
       </c>
       <c r="F107" s="4">
-        <v>93.8</v>
+        <v>93.7</v>
       </c>
       <c r="G107" s="4">
         <v>103.5</v>
@@ -7120,7 +7123,7 @@
         <v>103.7</v>
       </c>
       <c r="F108" s="4">
-        <v>94.2</v>
+        <v>94.1</v>
       </c>
       <c r="G108" s="4">
         <v>103.7</v>
@@ -7129,7 +7132,7 @@
         <v>106.8</v>
       </c>
       <c r="I108" s="4">
-        <v>95.9</v>
+        <v>95.8</v>
       </c>
       <c r="J108" s="4">
         <v>54.5</v>
@@ -7261,7 +7264,7 @@
         <v>105.7</v>
       </c>
       <c r="F111" s="4">
-        <v>96.9</v>
+        <v>96.8</v>
       </c>
       <c r="G111" s="4">
         <v>103.3</v>
@@ -7308,7 +7311,7 @@
         <v>105.9</v>
       </c>
       <c r="F112" s="4">
-        <v>97.9</v>
+        <v>97.8</v>
       </c>
       <c r="G112" s="4">
         <v>104.5</v>
@@ -7364,7 +7367,7 @@
         <v>110.8</v>
       </c>
       <c r="I113" s="4">
-        <v>99.7</v>
+        <v>99.6</v>
       </c>
       <c r="J113" s="4">
         <v>63.6</v>
@@ -7402,7 +7405,7 @@
         <v>107.8</v>
       </c>
       <c r="F114" s="4">
-        <v>98.9</v>
+        <v>98.8</v>
       </c>
       <c r="G114" s="4">
         <v>106.7</v>
@@ -7411,7 +7414,7 @@
         <v>111</v>
       </c>
       <c r="I114" s="4">
-        <v>101</v>
+        <v>100.9</v>
       </c>
       <c r="J114" s="4">
         <v>81.8</v>
@@ -7543,7 +7546,7 @@
         <v>112.2</v>
       </c>
       <c r="F117" s="4">
-        <v>101.3</v>
+        <v>101.2</v>
       </c>
       <c r="G117" s="4">
         <v>106</v>
@@ -7637,7 +7640,7 @@
         <v>109.5</v>
       </c>
       <c r="F119" s="4">
-        <v>102.7</v>
+        <v>102.6</v>
       </c>
       <c r="G119" s="4">
         <v>105.3</v>
@@ -7731,7 +7734,7 @@
         <v>109.6</v>
       </c>
       <c r="F121" s="4">
-        <v>104.2</v>
+        <v>104.1</v>
       </c>
       <c r="G121" s="4">
         <v>105.5</v>
@@ -7881,7 +7884,7 @@
         <v>114.5</v>
       </c>
       <c r="I124" s="4">
-        <v>106.9</v>
+        <v>106.8</v>
       </c>
       <c r="J124" s="4">
         <v>45.5</v>
@@ -7919,7 +7922,7 @@
         <v>111.9</v>
       </c>
       <c r="F125" s="4">
-        <v>106</v>
+        <v>105.9</v>
       </c>
       <c r="G125" s="4">
         <v>106.4</v>
@@ -8210,7 +8213,7 @@
         <v>119</v>
       </c>
       <c r="I131" s="4">
-        <v>109.3</v>
+        <v>109.2</v>
       </c>
       <c r="J131" s="4">
         <v>63.6</v>
@@ -8248,7 +8251,7 @@
         <v>115.7</v>
       </c>
       <c r="F132" s="4">
-        <v>107.3</v>
+        <v>107.2</v>
       </c>
       <c r="G132" s="4">
         <v>108</v>
@@ -8680,7 +8683,7 @@
         <v>118.6</v>
       </c>
       <c r="I141" s="4">
-        <v>111.5</v>
+        <v>111.6</v>
       </c>
       <c r="J141" s="4">
         <v>18.2</v>
@@ -9047,7 +9050,7 @@
         <v>111.4</v>
       </c>
       <c r="F149" s="4">
-        <v>109</v>
+        <v>108.9</v>
       </c>
       <c r="G149" s="4">
         <v>92.7</v>
@@ -9094,7 +9097,7 @@
         <v>109.4</v>
       </c>
       <c r="F150" s="4">
-        <v>108.1</v>
+        <v>108</v>
       </c>
       <c r="G150" s="4">
         <v>91.5</v>
@@ -9235,7 +9238,7 @@
         <v>105.7</v>
       </c>
       <c r="F153" s="4">
-        <v>106.1</v>
+        <v>106</v>
       </c>
       <c r="G153" s="4">
         <v>90</v>
@@ -9376,7 +9379,7 @@
         <v>102.5</v>
       </c>
       <c r="F156" s="4">
-        <v>104.5</v>
+        <v>104.4</v>
       </c>
       <c r="G156" s="4">
         <v>87.7</v>
@@ -9470,7 +9473,7 @@
         <v>99.3</v>
       </c>
       <c r="F158" s="4">
-        <v>103.2</v>
+        <v>103.1</v>
       </c>
       <c r="G158" s="4">
         <v>86.9</v>
@@ -9705,7 +9708,7 @@
         <v>96.7</v>
       </c>
       <c r="F163" s="4">
-        <v>99.7</v>
+        <v>99.6</v>
       </c>
       <c r="G163" s="4">
         <v>86.7</v>
@@ -9761,7 +9764,7 @@
         <v>100.8</v>
       </c>
       <c r="I164" s="4">
-        <v>101</v>
+        <v>100.9</v>
       </c>
       <c r="J164" s="4">
         <v>54.5</v>
@@ -9846,7 +9849,7 @@
         <v>96</v>
       </c>
       <c r="F166" s="4">
-        <v>97.3</v>
+        <v>97.2</v>
       </c>
       <c r="G166" s="4">
         <v>88.6</v>
@@ -10034,7 +10037,7 @@
         <v>93.3</v>
       </c>
       <c r="F170" s="4">
-        <v>94.8</v>
+        <v>94.7</v>
       </c>
       <c r="G170" s="4">
         <v>90.3</v>
@@ -10043,7 +10046,7 @@
         <v>97.3</v>
       </c>
       <c r="I170" s="4">
-        <v>96.4</v>
+        <v>96.3</v>
       </c>
       <c r="J170" s="4">
         <v>36.4</v>
@@ -10090,7 +10093,7 @@
         <v>97.3</v>
       </c>
       <c r="I171" s="4">
-        <v>95.4</v>
+        <v>95.3</v>
       </c>
       <c r="J171" s="4">
         <v>63.6</v>
@@ -10137,7 +10140,7 @@
         <v>95.8</v>
       </c>
       <c r="I172" s="4">
-        <v>95.1</v>
+        <v>95</v>
       </c>
       <c r="J172" s="4">
         <v>45.5</v>
@@ -10410,7 +10413,7 @@
         <v>93.2</v>
       </c>
       <c r="F178" s="4">
-        <v>91.1</v>
+        <v>91</v>
       </c>
       <c r="G178" s="4">
         <v>94.2</v>
@@ -10419,7 +10422,7 @@
         <v>97</v>
       </c>
       <c r="I178" s="4">
-        <v>92.6</v>
+        <v>92.5</v>
       </c>
       <c r="J178" s="4">
         <v>81.8</v>
@@ -10560,7 +10563,7 @@
         <v>99</v>
       </c>
       <c r="I181" s="4">
-        <v>91.8</v>
+        <v>91.7</v>
       </c>
       <c r="J181" s="4">
         <v>77.3</v>
@@ -10607,7 +10610,7 @@
         <v>99.9</v>
       </c>
       <c r="I182" s="4">
-        <v>92.1</v>
+        <v>92</v>
       </c>
       <c r="J182" s="4">
         <v>81.8</v>
@@ -10654,7 +10657,7 @@
         <v>99.5</v>
       </c>
       <c r="I183" s="4">
-        <v>92.4</v>
+        <v>92.3</v>
       </c>
       <c r="J183" s="4">
         <v>63.6</v>
@@ -10692,7 +10695,7 @@
         <v>96.2</v>
       </c>
       <c r="F184" s="4">
-        <v>90.7</v>
+        <v>90.6</v>
       </c>
       <c r="G184" s="4">
         <v>98.7</v>
@@ -10739,7 +10742,7 @@
         <v>97.2</v>
       </c>
       <c r="F185" s="4">
-        <v>90.6</v>
+        <v>90.5</v>
       </c>
       <c r="G185" s="4">
         <v>100.2</v>
@@ -10786,7 +10789,7 @@
         <v>97.5</v>
       </c>
       <c r="F186" s="4">
-        <v>91.1</v>
+        <v>91</v>
       </c>
       <c r="G186" s="4">
         <v>101.1</v>
@@ -10842,7 +10845,7 @@
         <v>99.5</v>
       </c>
       <c r="I187" s="4">
-        <v>92.1</v>
+        <v>92</v>
       </c>
       <c r="J187" s="4">
         <v>45.5</v>
@@ -10889,7 +10892,7 @@
         <v>101.7</v>
       </c>
       <c r="I188" s="4">
-        <v>92.8</v>
+        <v>92.7</v>
       </c>
       <c r="J188" s="4">
         <v>54.5</v>
@@ -11030,7 +11033,7 @@
         <v>101.9</v>
       </c>
       <c r="I191" s="4">
-        <v>92.7</v>
+        <v>92.6</v>
       </c>
       <c r="J191" s="4">
         <v>18.2</v>
@@ -11077,7 +11080,7 @@
         <v>102.2</v>
       </c>
       <c r="I192" s="4">
-        <v>92.7</v>
+        <v>92.6</v>
       </c>
       <c r="J192" s="4">
         <v>18.2</v>
@@ -11162,7 +11165,7 @@
         <v>97.8</v>
       </c>
       <c r="F194" s="4">
-        <v>91.3</v>
+        <v>91.2</v>
       </c>
       <c r="G194" s="4">
         <v>99.8</v>
@@ -11303,7 +11306,7 @@
         <v>98.6</v>
       </c>
       <c r="F197" s="4">
-        <v>92.2</v>
+        <v>92.1</v>
       </c>
       <c r="G197" s="4">
         <v>104</v>
@@ -11406,7 +11409,7 @@
         <v>103.1</v>
       </c>
       <c r="I199" s="4">
-        <v>94.3</v>
+        <v>94.2</v>
       </c>
       <c r="J199" s="4">
         <v>72.7</v>
@@ -11453,7 +11456,7 @@
         <v>104.4</v>
       </c>
       <c r="I200" s="4">
-        <v>95.5</v>
+        <v>95.4</v>
       </c>
       <c r="J200" s="4">
         <v>81.8</v>
@@ -11491,7 +11494,7 @@
         <v>99.8</v>
       </c>
       <c r="F201" s="4">
-        <v>94.1</v>
+        <v>94</v>
       </c>
       <c r="G201" s="4">
         <v>105.9</v>
@@ -11500,7 +11503,7 @@
         <v>104.1</v>
       </c>
       <c r="I201" s="4">
-        <v>95.6</v>
+        <v>95.5</v>
       </c>
       <c r="J201" s="4">
         <v>54.5</v>
@@ -11547,7 +11550,7 @@
         <v>105.2</v>
       </c>
       <c r="I202" s="4">
-        <v>95.8</v>
+        <v>95.7</v>
       </c>
       <c r="J202" s="4">
         <v>54.5</v>
@@ -11585,7 +11588,7 @@
         <v>101.9</v>
       </c>
       <c r="F203" s="4">
-        <v>94.7</v>
+        <v>94.6</v>
       </c>
       <c r="G203" s="4">
         <v>108.1</v>
@@ -11594,7 +11597,7 @@
         <v>106.3</v>
       </c>
       <c r="I203" s="4">
-        <v>96.3</v>
+        <v>96.2</v>
       </c>
       <c r="J203" s="4">
         <v>72.7</v>
@@ -11641,7 +11644,7 @@
         <v>106.1</v>
       </c>
       <c r="I204" s="4">
-        <v>96</v>
+        <v>95.9</v>
       </c>
       <c r="J204" s="4">
         <v>54.5</v>
@@ -11726,7 +11729,7 @@
         <v>102.5</v>
       </c>
       <c r="F206" s="4">
-        <v>95.8</v>
+        <v>95.7</v>
       </c>
       <c r="G206" s="4">
         <v>109.5</v>
@@ -11735,7 +11738,7 @@
         <v>107</v>
       </c>
       <c r="I206" s="4">
-        <v>97.3</v>
+        <v>97.2</v>
       </c>
       <c r="J206" s="4">
         <v>81.8</v>
@@ -11782,7 +11785,7 @@
         <v>107.5</v>
       </c>
       <c r="I207" s="4">
-        <v>97</v>
+        <v>96.9</v>
       </c>
       <c r="J207" s="4">
         <v>72.7</v>
@@ -11876,7 +11879,7 @@
         <v>110.2</v>
       </c>
       <c r="I209" s="4">
-        <v>99</v>
+        <v>98.9</v>
       </c>
       <c r="J209" s="4">
         <v>72.7</v>
@@ -11914,7 +11917,7 @@
         <v>105.7</v>
       </c>
       <c r="F210" s="4">
-        <v>97</v>
+        <v>96.9</v>
       </c>
       <c r="G210" s="4">
         <v>110.3</v>
@@ -11923,7 +11926,7 @@
         <v>110.2</v>
       </c>
       <c r="I210" s="4">
-        <v>98.4</v>
+        <v>98.3</v>
       </c>
       <c r="J210" s="4">
         <v>63.6</v>
@@ -11961,7 +11964,7 @@
         <v>107.2</v>
       </c>
       <c r="F211" s="4">
-        <v>97.9</v>
+        <v>97.8</v>
       </c>
       <c r="G211" s="4">
         <v>110.5</v>
@@ -11970,7 +11973,7 @@
         <v>111.8</v>
       </c>
       <c r="I211" s="4">
-        <v>99.3</v>
+        <v>99.2</v>
       </c>
       <c r="J211" s="4">
         <v>54.5</v>
@@ -12017,7 +12020,7 @@
         <v>112.4</v>
       </c>
       <c r="I212" s="4">
-        <v>99.7</v>
+        <v>99.6</v>
       </c>
       <c r="J212" s="4">
         <v>63.6</v>
@@ -12111,7 +12114,7 @@
         <v>111.1</v>
       </c>
       <c r="I214" s="4">
-        <v>101.8</v>
+        <v>101.7</v>
       </c>
       <c r="J214" s="4">
         <v>36.4</v>
@@ -12205,7 +12208,7 @@
         <v>112.9</v>
       </c>
       <c r="I216" s="4">
-        <v>103.4</v>
+        <v>103.3</v>
       </c>
       <c r="J216" s="4">
         <v>45.5</v>
@@ -12384,7 +12387,7 @@
         <v>106.4</v>
       </c>
       <c r="F220" s="4">
-        <v>102</v>
+        <v>101.9</v>
       </c>
       <c r="G220" s="4">
         <v>104.9</v>
@@ -12440,7 +12443,7 @@
         <v>108.8</v>
       </c>
       <c r="I221" s="4">
-        <v>103.6</v>
+        <v>103.5</v>
       </c>
       <c r="J221" s="4">
         <v>4.5</v>
@@ -12807,7 +12810,7 @@
         <v>98.3</v>
       </c>
       <c r="F229" s="4">
-        <v>95.9</v>
+        <v>96</v>
       </c>
       <c r="G229" s="4">
         <v>95.8</v>
@@ -13277,7 +13280,7 @@
         <v>98.6</v>
       </c>
       <c r="F239" s="4">
-        <v>91.6</v>
+        <v>91.7</v>
       </c>
       <c r="G239" s="4">
         <v>98.9</v>
@@ -13333,7 +13336,7 @@
         <v>103.1</v>
       </c>
       <c r="I240" s="4">
-        <v>92.2</v>
+        <v>92.3</v>
       </c>
       <c r="J240" s="4">
         <v>72.7</v>
@@ -13371,7 +13374,7 @@
         <v>99.5</v>
       </c>
       <c r="F241" s="4">
-        <v>91.3</v>
+        <v>91.4</v>
       </c>
       <c r="G241" s="4">
         <v>101.8</v>
@@ -13803,7 +13806,7 @@
         <v>111.2</v>
       </c>
       <c r="I250" s="4">
-        <v>94.5</v>
+        <v>94.4</v>
       </c>
       <c r="J250" s="4">
         <v>72.7</v>
@@ -13888,7 +13891,7 @@
         <v>107.7</v>
       </c>
       <c r="F252" s="4">
-        <v>93.1</v>
+        <v>93</v>
       </c>
       <c r="G252" s="4">
         <v>108.4</v>
@@ -14217,7 +14220,7 @@
         <v>108</v>
       </c>
       <c r="F259" s="4">
-        <v>94.3</v>
+        <v>94.2</v>
       </c>
       <c r="G259" s="4">
         <v>107.1</v>
@@ -14264,7 +14267,7 @@
         <v>107.9</v>
       </c>
       <c r="F260" s="4">
-        <v>94.9</v>
+        <v>94.8</v>
       </c>
       <c r="G260" s="4">
         <v>106.6</v>
@@ -14273,7 +14276,7 @@
         <v>112.8</v>
       </c>
       <c r="I260" s="4">
-        <v>96.4</v>
+        <v>96.3</v>
       </c>
       <c r="J260" s="4">
         <v>18.2</v>
@@ -14311,7 +14314,7 @@
         <v>106.4</v>
       </c>
       <c r="F261" s="4">
-        <v>94.3</v>
+        <v>94.2</v>
       </c>
       <c r="G261" s="4">
         <v>105.1</v>
@@ -14320,7 +14323,7 @@
         <v>111.3</v>
       </c>
       <c r="I261" s="4">
-        <v>95.8</v>
+        <v>95.7</v>
       </c>
       <c r="J261" s="4">
         <v>9.1</v>
@@ -14358,7 +14361,7 @@
         <v>105.4</v>
       </c>
       <c r="F262" s="4">
-        <v>94.1</v>
+        <v>94</v>
       </c>
       <c r="G262" s="4">
         <v>103.8</v>
@@ -14405,7 +14408,7 @@
         <v>104</v>
       </c>
       <c r="F263" s="4">
-        <v>94.2</v>
+        <v>94.1</v>
       </c>
       <c r="G263" s="4">
         <v>104.1</v>
@@ -14461,7 +14464,7 @@
         <v>108.4</v>
       </c>
       <c r="I264" s="4">
-        <v>95.4</v>
+        <v>95.3</v>
       </c>
       <c r="J264" s="4">
         <v>27.3</v>
@@ -14593,7 +14596,7 @@
         <v>99</v>
       </c>
       <c r="F267" s="4">
-        <v>93.3</v>
+        <v>93.2</v>
       </c>
       <c r="G267" s="4">
         <v>97.7</v>
@@ -14602,7 +14605,7 @@
         <v>103.5</v>
       </c>
       <c r="I267" s="4">
-        <v>95</v>
+        <v>94.9</v>
       </c>
       <c r="J267" s="4">
         <v>22.7</v>
@@ -14640,7 +14643,7 @@
         <v>98.4</v>
       </c>
       <c r="F268" s="4">
-        <v>93.3</v>
+        <v>93.2</v>
       </c>
       <c r="G268" s="4">
         <v>96.6</v>
@@ -14649,7 +14652,7 @@
         <v>103</v>
       </c>
       <c r="I268" s="4">
-        <v>95</v>
+        <v>94.9</v>
       </c>
       <c r="J268" s="4">
         <v>13.6</v>
@@ -14696,7 +14699,7 @@
         <v>101.9</v>
       </c>
       <c r="I269" s="4">
-        <v>94.3</v>
+        <v>94.2</v>
       </c>
       <c r="J269" s="4">
         <v>18.2</v>
@@ -14790,7 +14793,7 @@
         <v>101.7</v>
       </c>
       <c r="I271" s="4">
-        <v>93.7</v>
+        <v>93.6</v>
       </c>
       <c r="J271" s="4">
         <v>81.8</v>
@@ -14828,7 +14831,7 @@
         <v>98.3</v>
       </c>
       <c r="F272" s="4">
-        <v>91.5</v>
+        <v>91.4</v>
       </c>
       <c r="G272" s="4">
         <v>99.7</v>
@@ -14837,7 +14840,7 @@
         <v>102.8</v>
       </c>
       <c r="I272" s="4">
-        <v>93.2</v>
+        <v>93.1</v>
       </c>
       <c r="J272" s="4">
         <v>59.1</v>
@@ -14875,7 +14878,7 @@
         <v>99</v>
       </c>
       <c r="F273" s="4">
-        <v>91.2</v>
+        <v>91.1</v>
       </c>
       <c r="G273" s="4">
         <v>102.5</v>
@@ -14931,7 +14934,7 @@
         <v>103.9</v>
       </c>
       <c r="I274" s="4">
-        <v>92.9</v>
+        <v>92.8</v>
       </c>
       <c r="J274" s="4">
         <v>86.4</v>
@@ -14978,7 +14981,7 @@
         <v>106.7</v>
       </c>
       <c r="I275" s="4">
-        <v>92.3</v>
+        <v>92.2</v>
       </c>
       <c r="J275" s="4">
         <v>86.4</v>
@@ -15016,7 +15019,7 @@
         <v>101.6</v>
       </c>
       <c r="F276" s="4">
-        <v>90.5</v>
+        <v>90.4</v>
       </c>
       <c r="G276" s="4">
         <v>106</v>
@@ -15025,7 +15028,7 @@
         <v>106.1</v>
       </c>
       <c r="I276" s="4">
-        <v>92.3</v>
+        <v>92.2</v>
       </c>
       <c r="J276" s="4">
         <v>63.6</v>
@@ -15072,7 +15075,7 @@
         <v>106.6</v>
       </c>
       <c r="I277" s="4">
-        <v>92.7</v>
+        <v>92.6</v>
       </c>
       <c r="J277" s="4">
         <v>63.6</v>
@@ -15119,7 +15122,7 @@
         <v>107.8</v>
       </c>
       <c r="I278" s="4">
-        <v>92.4</v>
+        <v>92.3</v>
       </c>
       <c r="J278" s="4">
         <v>45.5</v>
@@ -15157,7 +15160,7 @@
         <v>103.7</v>
       </c>
       <c r="F279" s="4">
-        <v>91.4</v>
+        <v>91.3</v>
       </c>
       <c r="G279" s="4">
         <v>105.6</v>
@@ -15166,7 +15169,7 @@
         <v>108.3</v>
       </c>
       <c r="I279" s="4">
-        <v>93.3</v>
+        <v>93.2</v>
       </c>
       <c r="J279" s="4">
         <v>45.5</v>
@@ -15204,7 +15207,7 @@
         <v>103.6</v>
       </c>
       <c r="F280" s="4">
-        <v>91.6</v>
+        <v>91.5</v>
       </c>
       <c r="G280" s="4">
         <v>106.4</v>
@@ -15260,7 +15263,7 @@
         <v>109</v>
       </c>
       <c r="I281" s="4">
-        <v>93.8</v>
+        <v>93.7</v>
       </c>
       <c r="J281" s="4">
         <v>54.5</v>
@@ -15307,7 +15310,7 @@
         <v>108.1</v>
       </c>
       <c r="I282" s="4">
-        <v>94.5</v>
+        <v>94.4</v>
       </c>
       <c r="J282" s="4">
         <v>72.7</v>
@@ -15354,7 +15357,7 @@
         <v>108.7</v>
       </c>
       <c r="I283" s="4">
-        <v>94.7</v>
+        <v>94.6</v>
       </c>
       <c r="J283" s="4">
         <v>45.5</v>
@@ -15392,7 +15395,7 @@
         <v>105.1</v>
       </c>
       <c r="F284" s="4">
-        <v>93.1</v>
+        <v>93</v>
       </c>
       <c r="G284" s="4">
         <v>106.4</v>
@@ -15486,7 +15489,7 @@
         <v>104.3</v>
       </c>
       <c r="F286" s="4">
-        <v>93.5</v>
+        <v>93.4</v>
       </c>
       <c r="G286" s="4">
         <v>106.2</v>
@@ -15495,7 +15498,7 @@
         <v>108.9</v>
       </c>
       <c r="I286" s="4">
-        <v>95.5</v>
+        <v>95.4</v>
       </c>
       <c r="J286" s="4">
         <v>54.5</v>
@@ -15674,7 +15677,7 @@
         <v>105.9</v>
       </c>
       <c r="F290" s="4">
-        <v>96.5</v>
+        <v>96.4</v>
       </c>
       <c r="G290" s="4">
         <v>109</v>
@@ -15730,7 +15733,7 @@
         <v>112.5</v>
       </c>
       <c r="I291" s="4">
-        <v>98.6</v>
+        <v>98.5</v>
       </c>
       <c r="J291" s="4">
         <v>77.3</v>
@@ -15768,7 +15771,7 @@
         <v>110</v>
       </c>
       <c r="F292" s="4">
-        <v>97.6</v>
+        <v>97.5</v>
       </c>
       <c r="G292" s="4">
         <v>113.4</v>
@@ -15824,7 +15827,7 @@
         <v>114.3</v>
       </c>
       <c r="I293" s="4">
-        <v>99.9</v>
+        <v>99.8</v>
       </c>
       <c r="J293" s="4">
         <v>72.7</v>
@@ -15909,7 +15912,7 @@
         <v>112.9</v>
       </c>
       <c r="F295" s="4">
-        <v>100</v>
+        <v>99.9</v>
       </c>
       <c r="G295" s="4">
         <v>114.9</v>
@@ -15918,7 +15921,7 @@
         <v>118</v>
       </c>
       <c r="I295" s="4">
-        <v>102.1</v>
+        <v>102</v>
       </c>
       <c r="J295" s="4">
         <v>72.7</v>
@@ -16012,7 +16015,7 @@
         <v>117.8</v>
       </c>
       <c r="I297" s="4">
-        <v>102.3</v>
+        <v>102.2</v>
       </c>
       <c r="J297" s="4">
         <v>72.7</v>
@@ -16238,7 +16241,7 @@
         <v>114.9</v>
       </c>
       <c r="F302" s="4">
-        <v>102.9</v>
+        <v>102.8</v>
       </c>
       <c r="G302" s="4">
         <v>119.6</v>
@@ -16717,7 +16720,7 @@
         <v>121.6</v>
       </c>
       <c r="I312" s="4">
-        <v>107.6</v>
+        <v>107.5</v>
       </c>
       <c r="J312" s="4">
         <v>54.5</v>
@@ -16764,7 +16767,7 @@
         <v>120.9</v>
       </c>
       <c r="I313" s="4">
-        <v>106.8</v>
+        <v>106.7</v>
       </c>
       <c r="J313" s="4">
         <v>45.5</v>
@@ -16905,7 +16908,7 @@
         <v>122.5</v>
       </c>
       <c r="I316" s="4">
-        <v>107.6</v>
+        <v>107.5</v>
       </c>
       <c r="J316" s="4">
         <v>63.6</v>
@@ -17093,7 +17096,7 @@
         <v>125.3</v>
       </c>
       <c r="I320" s="4">
-        <v>109.4</v>
+        <v>109.5</v>
       </c>
       <c r="J320" s="4">
         <v>72.7</v>
@@ -17131,7 +17134,7 @@
         <v>120.3</v>
       </c>
       <c r="F321" s="4">
-        <v>107.2</v>
+        <v>107.3</v>
       </c>
       <c r="G321" s="4">
         <v>124.2</v>
@@ -17319,7 +17322,7 @@
         <v>121.7</v>
       </c>
       <c r="F325" s="4">
-        <v>109.8</v>
+        <v>109.9</v>
       </c>
       <c r="G325" s="4">
         <v>123.5</v>
@@ -17648,7 +17651,7 @@
         <v>122.3</v>
       </c>
       <c r="F332" s="4">
-        <v>111.2</v>
+        <v>111.3</v>
       </c>
       <c r="G332" s="4">
         <v>125.9</v>
@@ -17704,7 +17707,7 @@
         <v>127</v>
       </c>
       <c r="I333" s="4">
-        <v>113.7</v>
+        <v>113.8</v>
       </c>
       <c r="J333" s="4">
         <v>45.5</v>
@@ -17742,7 +17745,7 @@
         <v>122.7</v>
       </c>
       <c r="F334" s="4">
-        <v>112.3</v>
+        <v>112.4</v>
       </c>
       <c r="G334" s="4">
         <v>125.5</v>
@@ -17789,7 +17792,7 @@
         <v>123.3</v>
       </c>
       <c r="F335" s="4">
-        <v>112.3</v>
+        <v>112.4</v>
       </c>
       <c r="G335" s="4">
         <v>124.9</v>
@@ -17798,7 +17801,7 @@
         <v>128.6</v>
       </c>
       <c r="I335" s="4">
-        <v>114.5</v>
+        <v>114.6</v>
       </c>
       <c r="J335" s="4">
         <v>27.3</v>
@@ -17836,7 +17839,7 @@
         <v>123</v>
       </c>
       <c r="F336" s="4">
-        <v>112.6</v>
+        <v>112.7</v>
       </c>
       <c r="G336" s="4">
         <v>124.7</v>
@@ -17883,7 +17886,7 @@
         <v>122</v>
       </c>
       <c r="F337" s="4">
-        <v>113.2</v>
+        <v>113.3</v>
       </c>
       <c r="G337" s="4">
         <v>123</v>
@@ -17977,7 +17980,7 @@
         <v>121.9</v>
       </c>
       <c r="F339" s="4">
-        <v>113.4</v>
+        <v>113.5</v>
       </c>
       <c r="G339" s="4">
         <v>119.1</v>
@@ -17986,7 +17989,7 @@
         <v>127.6</v>
       </c>
       <c r="I339" s="4">
-        <v>115.6</v>
+        <v>115.7</v>
       </c>
       <c r="J339" s="4">
         <v>18.2</v>
@@ -18024,7 +18027,7 @@
         <v>122.8</v>
       </c>
       <c r="F340" s="4">
-        <v>113.8</v>
+        <v>113.9</v>
       </c>
       <c r="G340" s="4">
         <v>121.3</v>
@@ -18033,7 +18036,7 @@
         <v>128.5</v>
       </c>
       <c r="I340" s="4">
-        <v>116</v>
+        <v>116.1</v>
       </c>
       <c r="J340" s="4">
         <v>27.3</v>
@@ -18080,7 +18083,7 @@
         <v>127.3</v>
       </c>
       <c r="I341" s="4">
-        <v>117.4</v>
+        <v>117.5</v>
       </c>
       <c r="J341" s="4">
         <v>45.5</v>
@@ -18165,7 +18168,7 @@
         <v>121.2</v>
       </c>
       <c r="F343" s="4">
-        <v>114.3</v>
+        <v>114.4</v>
       </c>
       <c r="G343" s="4">
         <v>118.9</v>
@@ -18212,7 +18215,7 @@
         <v>121.4</v>
       </c>
       <c r="F344" s="4">
-        <v>114.7</v>
+        <v>114.8</v>
       </c>
       <c r="G344" s="4">
         <v>119.5</v>
@@ -18306,7 +18309,7 @@
         <v>119.8</v>
       </c>
       <c r="F346" s="4">
-        <v>112.8</v>
+        <v>112.9</v>
       </c>
       <c r="G346" s="4">
         <v>117.1</v>
@@ -18353,7 +18356,7 @@
         <v>120.1</v>
       </c>
       <c r="F347" s="4">
-        <v>112.5</v>
+        <v>112.6</v>
       </c>
       <c r="G347" s="4">
         <v>116.8</v>
@@ -18447,7 +18450,7 @@
         <v>117.1</v>
       </c>
       <c r="F349" s="4">
-        <v>111.9</v>
+        <v>112</v>
       </c>
       <c r="G349" s="4">
         <v>114.6</v>
@@ -18494,7 +18497,7 @@
         <v>113.4</v>
       </c>
       <c r="F350" s="4">
-        <v>110.6</v>
+        <v>110.7</v>
       </c>
       <c r="G350" s="4">
         <v>112.2</v>
@@ -18541,7 +18544,7 @@
         <v>112.4</v>
       </c>
       <c r="F351" s="4">
-        <v>110.2</v>
+        <v>110.3</v>
       </c>
       <c r="G351" s="4">
         <v>110.8</v>
@@ -18588,7 +18591,7 @@
         <v>108.8</v>
       </c>
       <c r="F352" s="4">
-        <v>109.5</v>
+        <v>109.6</v>
       </c>
       <c r="G352" s="4">
         <v>103.3</v>
@@ -18776,7 +18779,7 @@
         <v>83.5</v>
       </c>
       <c r="F356" s="4">
-        <v>97.6</v>
+        <v>97.5</v>
       </c>
       <c r="G356" s="4">
         <v>79.599999999999994</v>
@@ -18823,7 +18826,7 @@
         <v>83.1</v>
       </c>
       <c r="F357" s="4">
-        <v>95.9</v>
+        <v>95.8</v>
       </c>
       <c r="G357" s="4">
         <v>81.599999999999994</v>
@@ -18917,7 +18920,7 @@
         <v>86.3</v>
       </c>
       <c r="F359" s="4">
-        <v>91.7</v>
+        <v>91.6</v>
       </c>
       <c r="G359" s="4">
         <v>88</v>
@@ -18926,7 +18929,7 @@
         <v>86.6</v>
       </c>
       <c r="I359" s="4">
-        <v>92.5</v>
+        <v>92.4</v>
       </c>
       <c r="J359" s="4">
         <v>81.8</v>
@@ -18964,7 +18967,7 @@
         <v>87.9</v>
       </c>
       <c r="F360" s="4">
-        <v>90.7</v>
+        <v>90.6</v>
       </c>
       <c r="G360" s="4">
         <v>91.9</v>
@@ -18973,7 +18976,7 @@
         <v>89.5</v>
       </c>
       <c r="I360" s="4">
-        <v>91.8</v>
+        <v>91.7</v>
       </c>
       <c r="J360" s="4">
         <v>81.8</v>
@@ -19020,7 +19023,7 @@
         <v>91</v>
       </c>
       <c r="I361" s="4">
-        <v>90.4</v>
+        <v>90.3</v>
       </c>
       <c r="J361" s="4">
         <v>68.2</v>
@@ -19105,7 +19108,7 @@
         <v>93.2</v>
       </c>
       <c r="F363" s="4">
-        <v>89.6</v>
+        <v>89.5</v>
       </c>
       <c r="G363" s="4">
         <v>98.3</v>
@@ -19114,7 +19117,7 @@
         <v>96.2</v>
       </c>
       <c r="I363" s="4">
-        <v>90.7</v>
+        <v>90.6</v>
       </c>
       <c r="J363" s="4">
         <v>81.8</v>
@@ -19152,7 +19155,7 @@
         <v>95.3</v>
       </c>
       <c r="F364" s="4">
-        <v>89.1</v>
+        <v>89</v>
       </c>
       <c r="G364" s="4">
         <v>100.9</v>
@@ -19255,7 +19258,7 @@
         <v>101.7</v>
       </c>
       <c r="I366" s="4">
-        <v>90.7</v>
+        <v>90.6</v>
       </c>
       <c r="J366" s="4">
         <v>72.7</v>
@@ -19349,7 +19352,7 @@
         <v>105.6</v>
       </c>
       <c r="I368" s="4">
-        <v>91.5</v>
+        <v>91.4</v>
       </c>
       <c r="J368" s="4">
         <v>72.7</v>
@@ -19396,7 +19399,7 @@
         <v>107.1</v>
       </c>
       <c r="I369" s="4">
-        <v>91.9</v>
+        <v>91.8</v>
       </c>
       <c r="J369" s="4">
         <v>90.9</v>
@@ -19481,7 +19484,7 @@
         <v>104.6</v>
       </c>
       <c r="F371" s="4">
-        <v>91.7</v>
+        <v>91.6</v>
       </c>
       <c r="G371" s="4">
         <v>107.8</v>
@@ -19490,7 +19493,7 @@
         <v>108.2</v>
       </c>
       <c r="I371" s="4">
-        <v>92.6</v>
+        <v>92.5</v>
       </c>
       <c r="J371" s="4">
         <v>90.9</v>
@@ -19584,7 +19587,7 @@
         <v>109.6</v>
       </c>
       <c r="I373" s="4">
-        <v>94</v>
+        <v>93.9</v>
       </c>
       <c r="J373" s="4">
         <v>54.5</v>
@@ -19622,7 +19625,7 @@
         <v>106.1</v>
       </c>
       <c r="F374" s="4">
-        <v>92.7</v>
+        <v>92.6</v>
       </c>
       <c r="G374" s="4">
         <v>109</v>
@@ -19669,7 +19672,7 @@
         <v>106.9</v>
       </c>
       <c r="F375" s="4">
-        <v>93</v>
+        <v>92.9</v>
       </c>
       <c r="G375" s="4">
         <v>108.3</v>
@@ -19678,7 +19681,7 @@
         <v>110.6</v>
       </c>
       <c r="I375" s="4">
-        <v>93.9</v>
+        <v>93.8</v>
       </c>
       <c r="J375" s="4">
         <v>54.5</v>
@@ -19716,7 +19719,7 @@
         <v>106.4</v>
       </c>
       <c r="F376" s="4">
-        <v>93.8</v>
+        <v>93.7</v>
       </c>
       <c r="G376" s="4">
         <v>108.1</v>
@@ -19763,7 +19766,7 @@
         <v>108.4</v>
       </c>
       <c r="F377" s="4">
-        <v>93.7</v>
+        <v>93.6</v>
       </c>
       <c r="G377" s="4">
         <v>109.2</v>
@@ -19810,7 +19813,7 @@
         <v>108.7</v>
       </c>
       <c r="F378" s="4">
-        <v>94</v>
+        <v>93.9</v>
       </c>
       <c r="G378" s="4">
         <v>109.9</v>
@@ -19819,7 +19822,7 @@
         <v>112.4</v>
       </c>
       <c r="I378" s="4">
-        <v>94.9</v>
+        <v>94.8</v>
       </c>
       <c r="J378" s="4">
         <v>63.6</v>
@@ -19857,7 +19860,7 @@
         <v>108.5</v>
       </c>
       <c r="F379" s="4">
-        <v>94.2</v>
+        <v>94.1</v>
       </c>
       <c r="G379" s="4">
         <v>110.8</v>
@@ -19904,7 +19907,7 @@
         <v>110</v>
       </c>
       <c r="F380" s="4">
-        <v>94.9</v>
+        <v>94.8</v>
       </c>
       <c r="G380" s="4">
         <v>111.7</v>
@@ -19951,7 +19954,7 @@
         <v>102.1</v>
       </c>
       <c r="F381" s="4">
-        <v>92.7</v>
+        <v>92.6</v>
       </c>
       <c r="G381" s="4">
         <v>109.1</v>
@@ -19960,7 +19963,7 @@
         <v>103.2</v>
       </c>
       <c r="I381" s="4">
-        <v>92.7</v>
+        <v>92.6</v>
       </c>
       <c r="J381" s="4">
         <v>45.5</v>
@@ -19998,7 +20001,7 @@
         <v>100.9</v>
       </c>
       <c r="F382" s="4">
-        <v>93.7</v>
+        <v>93.6</v>
       </c>
       <c r="G382" s="4">
         <v>103.2</v>
@@ -20045,7 +20048,7 @@
         <v>103.5</v>
       </c>
       <c r="F383" s="4">
-        <v>94.4</v>
+        <v>94.3</v>
       </c>
       <c r="G383" s="4">
         <v>103.3</v>
@@ -20054,7 +20057,7 @@
         <v>104.2</v>
       </c>
       <c r="I383" s="4">
-        <v>94.6</v>
+        <v>94.5</v>
       </c>
       <c r="J383" s="4">
         <v>36.4</v>
@@ -20101,7 +20104,7 @@
         <v>107.7</v>
       </c>
       <c r="I384" s="4">
-        <v>94.7</v>
+        <v>94.6</v>
       </c>
       <c r="J384" s="4">
         <v>45.5</v>
@@ -20139,7 +20142,7 @@
         <v>106.9</v>
       </c>
       <c r="F385" s="4">
-        <v>94.9</v>
+        <v>94.8</v>
       </c>
       <c r="G385" s="4">
         <v>109.5</v>
@@ -20148,7 +20151,7 @@
         <v>108.8</v>
       </c>
       <c r="I385" s="4">
-        <v>95.1</v>
+        <v>95</v>
       </c>
       <c r="J385" s="4">
         <v>72.7</v>
@@ -20195,7 +20198,7 @@
         <v>110</v>
       </c>
       <c r="I386" s="4">
-        <v>96</v>
+        <v>95.9</v>
       </c>
       <c r="J386" s="4">
         <v>77.3</v>
@@ -20233,7 +20236,7 @@
         <v>108.8</v>
       </c>
       <c r="F387" s="4">
-        <v>96.7</v>
+        <v>96.6</v>
       </c>
       <c r="G387" s="4">
         <v>107.6</v>
@@ -20242,7 +20245,7 @@
         <v>110.5</v>
       </c>
       <c r="I387" s="4">
-        <v>96.9</v>
+        <v>96.8</v>
       </c>
       <c r="J387" s="4">
         <v>36.4</v>
@@ -20280,7 +20283,7 @@
         <v>110.4</v>
       </c>
       <c r="F388" s="4">
-        <v>96.3</v>
+        <v>96.2</v>
       </c>
       <c r="G388" s="4">
         <v>108</v>
@@ -20289,7 +20292,7 @@
         <v>112.1</v>
       </c>
       <c r="I388" s="4">
-        <v>96.8</v>
+        <v>96.7</v>
       </c>
       <c r="J388" s="4">
         <v>45.5</v>
@@ -20327,7 +20330,7 @@
         <v>108.9</v>
       </c>
       <c r="F389" s="4">
-        <v>96.5</v>
+        <v>96.4</v>
       </c>
       <c r="G389" s="4">
         <v>107.8</v>
@@ -20374,7 +20377,7 @@
         <v>111</v>
       </c>
       <c r="F390" s="4">
-        <v>97.2</v>
+        <v>97.1</v>
       </c>
       <c r="G390" s="4">
         <v>108.4</v>
@@ -20383,7 +20386,7 @@
         <v>112.9</v>
       </c>
       <c r="I390" s="4">
-        <v>97.9</v>
+        <v>97.8</v>
       </c>
       <c r="J390" s="4">
         <v>63.6</v>
@@ -20421,7 +20424,7 @@
         <v>111.1</v>
       </c>
       <c r="F391" s="4">
-        <v>96.6</v>
+        <v>96.5</v>
       </c>
       <c r="G391" s="4">
         <v>109.3</v>
@@ -20468,7 +20471,7 @@
         <v>112</v>
       </c>
       <c r="F392" s="4">
-        <v>97.8</v>
+        <v>97.7</v>
       </c>
       <c r="G392" s="4">
         <v>110.8</v>
@@ -20562,7 +20565,7 @@
         <v>111.8</v>
       </c>
       <c r="F394" s="4">
-        <v>98.7</v>
+        <v>98.6</v>
       </c>
       <c r="G394" s="4">
         <v>110.2</v>
@@ -20609,7 +20612,7 @@
         <v>111.6</v>
       </c>
       <c r="F395" s="4">
-        <v>98.3</v>
+        <v>98.2</v>
       </c>
       <c r="G395" s="4">
         <v>109.4</v>
@@ -20618,7 +20621,7 @@
         <v>113.5</v>
       </c>
       <c r="I395" s="4">
-        <v>98.8</v>
+        <v>98.7</v>
       </c>
       <c r="J395" s="4">
         <v>54.5</v>
@@ -20656,7 +20659,7 @@
         <v>109.3</v>
       </c>
       <c r="F396" s="4">
-        <v>98.2</v>
+        <v>98.1</v>
       </c>
       <c r="G396" s="4">
         <v>108</v>
@@ -20665,7 +20668,7 @@
         <v>111.2</v>
       </c>
       <c r="I396" s="4">
-        <v>98.7</v>
+        <v>98.6</v>
       </c>
       <c r="J396" s="4">
         <v>22.7</v>
@@ -20703,7 +20706,7 @@
         <v>108.7</v>
       </c>
       <c r="F397" s="4">
-        <v>97.4</v>
+        <v>97.3</v>
       </c>
       <c r="G397" s="4">
         <v>107.4</v>
@@ -20712,7 +20715,7 @@
         <v>110.6</v>
       </c>
       <c r="I397" s="4">
-        <v>97.8</v>
+        <v>97.7</v>
       </c>
       <c r="J397" s="4">
         <v>40.9</v>
@@ -20750,7 +20753,7 @@
         <v>108.5</v>
       </c>
       <c r="F398" s="4">
-        <v>97.4</v>
+        <v>97.3</v>
       </c>
       <c r="G398" s="4">
         <v>107.3</v>
@@ -20891,7 +20894,7 @@
         <v>106.4</v>
       </c>
       <c r="F401" s="4">
-        <v>97.3</v>
+        <v>97.2</v>
       </c>
       <c r="G401" s="4">
         <v>106.2</v>
@@ -20900,7 +20903,7 @@
         <v>108.2</v>
       </c>
       <c r="I401" s="4">
-        <v>97.5</v>
+        <v>97.4</v>
       </c>
       <c r="J401" s="4">
         <v>27.3</v>
@@ -20947,7 +20950,7 @@
         <v>109.6</v>
       </c>
       <c r="I402" s="4">
-        <v>97.4</v>
+        <v>97.3</v>
       </c>
       <c r="J402" s="4">
         <v>81.8</v>
@@ -20985,7 +20988,7 @@
         <v>108</v>
       </c>
       <c r="F403" s="4">
-        <v>96.7</v>
+        <v>96.6</v>
       </c>
       <c r="G403" s="4">
         <v>110.1</v>
@@ -21032,7 +21035,7 @@
         <v>109</v>
       </c>
       <c r="F404" s="4">
-        <v>96.3</v>
+        <v>96.2</v>
       </c>
       <c r="G404" s="4">
         <v>113.6</v>
@@ -21041,7 +21044,7 @@
         <v>110.7</v>
       </c>
       <c r="I404" s="4">
-        <v>96.3</v>
+        <v>96.2</v>
       </c>
       <c r="J404" s="4">
         <v>81.8</v>
@@ -21079,7 +21082,7 @@
         <v>110.7</v>
       </c>
       <c r="F405" s="4">
-        <v>96.4</v>
+        <v>96.3</v>
       </c>
       <c r="G405" s="4">
         <v>115.5</v>
@@ -21088,7 +21091,7 @@
         <v>112.5</v>
       </c>
       <c r="I405" s="4">
-        <v>96.4</v>
+        <v>96.3</v>
       </c>
       <c r="J405" s="4">
         <v>100</v>
@@ -21126,7 +21129,7 @@
         <v>111.3</v>
       </c>
       <c r="F406" s="4">
-        <v>96.3</v>
+        <v>96.2</v>
       </c>
       <c r="G406" s="4">
         <v>117.1</v>
@@ -21173,7 +21176,7 @@
         <v>112.8</v>
       </c>
       <c r="F407" s="4">
-        <v>97.1</v>
+        <v>97</v>
       </c>
       <c r="G407" s="4">
         <v>119.1</v>
@@ -21182,7 +21185,7 @@
         <v>114.5</v>
       </c>
       <c r="I407" s="4">
-        <v>97</v>
+        <v>96.9</v>
       </c>
       <c r="J407" s="4">
         <v>100</v>
@@ -21220,7 +21223,7 @@
         <v>112.5</v>
       </c>
       <c r="F408" s="4">
-        <v>97.6</v>
+        <v>97.5</v>
       </c>
       <c r="G408" s="4">
         <v>117.7</v>
@@ -21314,7 +21317,7 @@
         <v>114.6</v>
       </c>
       <c r="F410" s="4">
-        <v>98.7</v>
+        <v>98.6</v>
       </c>
       <c r="G410" s="4">
         <v>119.1</v>
@@ -21323,7 +21326,7 @@
         <v>116.4</v>
       </c>
       <c r="I410" s="4">
-        <v>98.4</v>
+        <v>98.3</v>
       </c>
       <c r="J410" s="4">
         <v>72.7</v>
@@ -21361,7 +21364,7 @@
         <v>115.3</v>
       </c>
       <c r="F411" s="4">
-        <v>99.2</v>
+        <v>99.1</v>
       </c>
       <c r="G411" s="4">
         <v>121.1</v>
@@ -21370,7 +21373,7 @@
         <v>117.1</v>
       </c>
       <c r="I411" s="4">
-        <v>98.8</v>
+        <v>98.7</v>
       </c>
       <c r="J411" s="4">
         <v>95.5</v>
@@ -21408,7 +21411,7 @@
         <v>116</v>
       </c>
       <c r="F412" s="4">
-        <v>99.6</v>
+        <v>99.5</v>
       </c>
       <c r="G412" s="4">
         <v>120.5</v>
@@ -21455,7 +21458,7 @@
         <v>117.1</v>
       </c>
       <c r="F413" s="4">
-        <v>100.5</v>
+        <v>100.4</v>
       </c>
       <c r="G413" s="4">
         <v>122.3</v>
@@ -21464,7 +21467,7 @@
         <v>119</v>
       </c>
       <c r="I413" s="4">
-        <v>100.1</v>
+        <v>100</v>
       </c>
       <c r="J413" s="4">
         <v>100</v>
@@ -21549,7 +21552,7 @@
         <v>118.6</v>
       </c>
       <c r="F415" s="4">
-        <v>102.6</v>
+        <v>102.5</v>
       </c>
       <c r="G415" s="4">
         <v>121.9</v>
@@ -21558,7 +21561,7 @@
         <v>120.5</v>
       </c>
       <c r="I415" s="4">
-        <v>102.3</v>
+        <v>102.2</v>
       </c>
       <c r="J415" s="4">
         <v>72.7</v>
@@ -21596,7 +21599,7 @@
         <v>118.4</v>
       </c>
       <c r="F416" s="4">
-        <v>102.8</v>
+        <v>102.7</v>
       </c>
       <c r="G416" s="4">
         <v>118.5</v>
@@ -21643,7 +21646,7 @@
         <v>120.4</v>
       </c>
       <c r="F417" s="4">
-        <v>103.4</v>
+        <v>103.3</v>
       </c>
       <c r="G417" s="4">
         <v>118.2</v>
@@ -21652,7 +21655,7 @@
         <v>122.6</v>
       </c>
       <c r="I417" s="4">
-        <v>103.2</v>
+        <v>103.1</v>
       </c>
       <c r="J417" s="4">
         <v>36.4</v>
@@ -21690,7 +21693,7 @@
         <v>116.3</v>
       </c>
       <c r="F418" s="4">
-        <v>103.5</v>
+        <v>103.4</v>
       </c>
       <c r="G418" s="4">
         <v>114.9</v>
@@ -21737,7 +21740,7 @@
         <v>116.8</v>
       </c>
       <c r="F419" s="4">
-        <v>105.6</v>
+        <v>105.5</v>
       </c>
       <c r="G419" s="4">
         <v>114.3</v>
@@ -21784,7 +21787,7 @@
         <v>115.6</v>
       </c>
       <c r="F420" s="4">
-        <v>105.6</v>
+        <v>105.5</v>
       </c>
       <c r="G420" s="4">
         <v>114.2</v>
@@ -21793,7 +21796,7 @@
         <v>117.4</v>
       </c>
       <c r="I420" s="4">
-        <v>106.8</v>
+        <v>106.7</v>
       </c>
       <c r="J420" s="4">
         <v>27.3</v>
@@ -21831,7 +21834,7 @@
         <v>116.2</v>
       </c>
       <c r="F421" s="4">
-        <v>105.8</v>
+        <v>105.7</v>
       </c>
       <c r="G421" s="4">
         <v>115.8</v>
@@ -21887,7 +21890,7 @@
         <v>117.1</v>
       </c>
       <c r="I422" s="4">
-        <v>106.5</v>
+        <v>106.4</v>
       </c>
       <c r="J422" s="4">
         <v>72.7</v>
@@ -21925,7 +21928,7 @@
         <v>116.9</v>
       </c>
       <c r="F423" s="4">
-        <v>105.5</v>
+        <v>105.4</v>
       </c>
       <c r="G423" s="4">
         <v>116.1</v>
@@ -21934,7 +21937,7 @@
         <v>118.7</v>
       </c>
       <c r="I423" s="4">
-        <v>106.7</v>
+        <v>106.6</v>
       </c>
       <c r="J423" s="4">
         <v>59.1</v>
@@ -21981,7 +21984,7 @@
         <v>118.4</v>
       </c>
       <c r="I424" s="4">
-        <v>106.5</v>
+        <v>106.4</v>
       </c>
       <c r="J424" s="4">
         <v>36.4</v>
@@ -22028,7 +22031,7 @@
         <v>117.8</v>
       </c>
       <c r="I425" s="4">
-        <v>106.4</v>
+        <v>106.3</v>
       </c>
       <c r="J425" s="4">
         <v>63.6</v>
@@ -22066,7 +22069,7 @@
         <v>116.2</v>
       </c>
       <c r="F426" s="4">
-        <v>105</v>
+        <v>104.9</v>
       </c>
       <c r="G426" s="4">
         <v>115.4</v>
@@ -22075,7 +22078,7 @@
         <v>118</v>
       </c>
       <c r="I426" s="4">
-        <v>106</v>
+        <v>105.9</v>
       </c>
       <c r="J426" s="4">
         <v>54.5</v>
@@ -22160,7 +22163,7 @@
         <v>116.7</v>
       </c>
       <c r="F428" s="4">
-        <v>105.3</v>
+        <v>105.2</v>
       </c>
       <c r="G428" s="4">
         <v>115.1</v>
@@ -22169,7 +22172,7 @@
         <v>117.6</v>
       </c>
       <c r="I428" s="4">
-        <v>106.2</v>
+        <v>106.1</v>
       </c>
       <c r="J428" s="4">
         <v>54.5</v>
@@ -22254,7 +22257,7 @@
         <v>117.2</v>
       </c>
       <c r="F430" s="4">
-        <v>105.3</v>
+        <v>105.2</v>
       </c>
       <c r="G430" s="4">
         <v>116.5</v>
@@ -22301,7 +22304,7 @@
         <v>116.4</v>
       </c>
       <c r="F431" s="4">
-        <v>105</v>
+        <v>104.9</v>
       </c>
       <c r="G431" s="4">
         <v>117.7</v>
@@ -22310,7 +22313,7 @@
         <v>118.2</v>
       </c>
       <c r="I431" s="4">
-        <v>104.2</v>
+        <v>104.1</v>
       </c>
       <c r="J431" s="4">
         <v>81.8</v>
@@ -22348,7 +22351,7 @@
         <v>117.2</v>
       </c>
       <c r="F432" s="4">
-        <v>104.5</v>
+        <v>104.4</v>
       </c>
       <c r="G432" s="4">
         <v>117.2</v>
@@ -22395,7 +22398,7 @@
         <v>117</v>
       </c>
       <c r="F433" s="4">
-        <v>104.9</v>
+        <v>104.8</v>
       </c>
       <c r="G433" s="4">
         <v>115.7</v>
@@ -22442,7 +22445,7 @@
         <v>116.1</v>
       </c>
       <c r="F434" s="4">
-        <v>104.6</v>
+        <v>104.5</v>
       </c>
       <c r="G434" s="4">
         <v>114.9</v>
@@ -22498,7 +22501,7 @@
         <v>118.8</v>
       </c>
       <c r="I435" s="4">
-        <v>104.2</v>
+        <v>104.1</v>
       </c>
       <c r="J435" s="4">
         <v>31.8</v>
@@ -22536,7 +22539,7 @@
         <v>116.7</v>
       </c>
       <c r="F436" s="4">
-        <v>105.2</v>
+        <v>105.1</v>
       </c>
       <c r="G436" s="4">
         <v>114.1</v>
@@ -22545,7 +22548,7 @@
         <v>118.5</v>
       </c>
       <c r="I436" s="4">
-        <v>104.2</v>
+        <v>104.1</v>
       </c>
       <c r="J436" s="4">
         <v>54.5</v>
@@ -22583,7 +22586,7 @@
         <v>116</v>
       </c>
       <c r="F437" s="4">
-        <v>105.3</v>
+        <v>105.2</v>
       </c>
       <c r="G437" s="4">
         <v>113</v>
@@ -22592,7 +22595,7 @@
         <v>117.8</v>
       </c>
       <c r="I437" s="4">
-        <v>104.2</v>
+        <v>104.1</v>
       </c>
       <c r="J437" s="4">
         <v>36.4</v>
@@ -22630,7 +22633,7 @@
         <v>115.1</v>
       </c>
       <c r="F438" s="4">
-        <v>105.1</v>
+        <v>105</v>
       </c>
       <c r="G438" s="4">
         <v>111.4</v>
@@ -22639,7 +22642,7 @@
         <v>116.8</v>
       </c>
       <c r="I438" s="4">
-        <v>105.1</v>
+        <v>105</v>
       </c>
       <c r="J438" s="4">
         <v>36.4</v>
@@ -22677,7 +22680,7 @@
         <v>116.5</v>
       </c>
       <c r="F439" s="4">
-        <v>104.8</v>
+        <v>104.7</v>
       </c>
       <c r="G439" s="4">
         <v>111.9</v>
@@ -22686,7 +22689,7 @@
         <v>118.3</v>
       </c>
       <c r="I439" s="4">
-        <v>103.8</v>
+        <v>103.7</v>
       </c>
       <c r="J439" s="4">
         <v>45.5</v>
@@ -22724,7 +22727,7 @@
         <v>115.4</v>
       </c>
       <c r="F440" s="4">
-        <v>104.9</v>
+        <v>104.8</v>
       </c>
       <c r="G440" s="4">
         <v>109.7</v>
@@ -22733,7 +22736,7 @@
         <v>117.2</v>
       </c>
       <c r="I440" s="4">
-        <v>103.9</v>
+        <v>103.8</v>
       </c>
       <c r="J440" s="4">
         <v>27.3</v>
@@ -22771,7 +22774,7 @@
         <v>115.7</v>
       </c>
       <c r="F441" s="4">
-        <v>104.6</v>
+        <v>104.5</v>
       </c>
       <c r="G441" s="4">
         <v>109.9</v>
@@ -22780,7 +22783,7 @@
         <v>117.5</v>
       </c>
       <c r="I441" s="4">
-        <v>103.5</v>
+        <v>103.4</v>
       </c>
       <c r="J441" s="4">
         <v>45.5</v>
@@ -22818,7 +22821,7 @@
         <v>115.4</v>
       </c>
       <c r="F442" s="4">
-        <v>104.5</v>
+        <v>104.4</v>
       </c>
       <c r="G442" s="4">
         <v>110</v>
@@ -22827,7 +22830,7 @@
         <v>117.2</v>
       </c>
       <c r="I442" s="4">
-        <v>103.5</v>
+        <v>103.4</v>
       </c>
       <c r="J442" s="4">
         <v>54.5</v>
@@ -22865,7 +22868,7 @@
         <v>115.1</v>
       </c>
       <c r="F443" s="4">
-        <v>103.7</v>
+        <v>103.6</v>
       </c>
       <c r="G443" s="4">
         <v>110.1</v>
@@ -22874,7 +22877,7 @@
         <v>116.9</v>
       </c>
       <c r="I443" s="4">
-        <v>102.7</v>
+        <v>102.6</v>
       </c>
       <c r="J443" s="4">
         <v>72.7</v>
@@ -22912,7 +22915,7 @@
         <v>115.4</v>
       </c>
       <c r="F444" s="4">
-        <v>104.5</v>
+        <v>104.4</v>
       </c>
       <c r="G444" s="4">
         <v>110.3</v>
@@ -22921,7 +22924,7 @@
         <v>117.2</v>
       </c>
       <c r="I444" s="4">
-        <v>103.5</v>
+        <v>103.4</v>
       </c>
       <c r="J444" s="4">
         <v>63.6</v>
@@ -22959,7 +22962,7 @@
         <v>115.9</v>
       </c>
       <c r="F445" s="4">
-        <v>104.5</v>
+        <v>104.4</v>
       </c>
       <c r="G445" s="4">
         <v>110.5</v>
@@ -22968,7 +22971,7 @@
         <v>117.7</v>
       </c>
       <c r="I445" s="4">
-        <v>103.4</v>
+        <v>103.3</v>
       </c>
       <c r="J445" s="4">
         <v>59.1</v>
@@ -23006,7 +23009,7 @@
         <v>116.2</v>
       </c>
       <c r="F446" s="4">
-        <v>104.6</v>
+        <v>104.5</v>
       </c>
       <c r="G446" s="4">
         <v>110.5</v>
@@ -23015,7 +23018,7 @@
         <v>118</v>
       </c>
       <c r="I446" s="4">
-        <v>103.6</v>
+        <v>103.5</v>
       </c>
       <c r="J446" s="4">
         <v>36.4</v>
@@ -23053,7 +23056,7 @@
         <v>116.7</v>
       </c>
       <c r="F447" s="4">
-        <v>105.1</v>
+        <v>105</v>
       </c>
       <c r="G447" s="4">
         <v>110.6</v>
@@ -23062,7 +23065,7 @@
         <v>118.5</v>
       </c>
       <c r="I447" s="4">
-        <v>104</v>
+        <v>103.9</v>
       </c>
       <c r="J447" s="4">
         <v>63.6</v>
@@ -23100,7 +23103,7 @@
         <v>117.4</v>
       </c>
       <c r="F448" s="4">
-        <v>105.2</v>
+        <v>105.1</v>
       </c>
       <c r="G448" s="4">
         <v>111.8</v>
@@ -23109,7 +23112,7 @@
         <v>119.2</v>
       </c>
       <c r="I448" s="4">
-        <v>104.1</v>
+        <v>104</v>
       </c>
       <c r="J448" s="4">
         <v>81.8</v>
@@ -23147,7 +23150,7 @@
         <v>119.1</v>
       </c>
       <c r="F449" s="4">
-        <v>105.5</v>
+        <v>105.4</v>
       </c>
       <c r="G449" s="4">
         <v>113.2</v>
@@ -23156,7 +23159,7 @@
         <v>121</v>
       </c>
       <c r="I449" s="4">
-        <v>104.4</v>
+        <v>104.3</v>
       </c>
       <c r="J449" s="4">
         <v>72.7</v>
@@ -23194,7 +23197,7 @@
         <v>119.2</v>
       </c>
       <c r="F450" s="4">
-        <v>106</v>
+        <v>105.9</v>
       </c>
       <c r="G450" s="4">
         <v>115.2</v>
@@ -23203,7 +23206,7 @@
         <v>121</v>
       </c>
       <c r="I450" s="4">
-        <v>105</v>
+        <v>104.9</v>
       </c>
       <c r="J450" s="4">
         <v>81.8</v>
@@ -23241,7 +23244,7 @@
         <v>118.7</v>
       </c>
       <c r="F451" s="4">
-        <v>106.4</v>
+        <v>106.3</v>
       </c>
       <c r="G451" s="4">
         <v>115.8</v>
@@ -23250,7 +23253,7 @@
         <v>120.6</v>
       </c>
       <c r="I451" s="4">
-        <v>105.3</v>
+        <v>105.2</v>
       </c>
       <c r="J451" s="4">
         <v>90.9</v>
@@ -23288,7 +23291,7 @@
         <v>119.4</v>
       </c>
       <c r="F452" s="4">
-        <v>107</v>
+        <v>106.9</v>
       </c>
       <c r="G452" s="4">
         <v>115.5</v>
@@ -23297,7 +23300,7 @@
         <v>121.2</v>
       </c>
       <c r="I452" s="4">
-        <v>105.9</v>
+        <v>105.8</v>
       </c>
       <c r="J452" s="4">
         <v>72.7</v>
@@ -23335,7 +23338,7 @@
         <v>119.5</v>
       </c>
       <c r="F453" s="4">
-        <v>107.7</v>
+        <v>107.6</v>
       </c>
       <c r="G453" s="4">
         <v>116.1</v>
@@ -23344,7 +23347,7 @@
         <v>121.4</v>
       </c>
       <c r="I453" s="4">
-        <v>106.6</v>
+        <v>106.5</v>
       </c>
       <c r="J453" s="4">
         <v>63.6</v>
@@ -23382,7 +23385,7 @@
         <v>120.7</v>
       </c>
       <c r="F454" s="4">
-        <v>108.1</v>
+        <v>108</v>
       </c>
       <c r="G454" s="4">
         <v>115.7</v>
@@ -23391,7 +23394,7 @@
         <v>122.5</v>
       </c>
       <c r="I454" s="4">
-        <v>107.1</v>
+        <v>107</v>
       </c>
       <c r="J454" s="4">
         <v>50</v>
@@ -23429,7 +23432,7 @@
         <v>120.6</v>
       </c>
       <c r="F455" s="4">
-        <v>108</v>
+        <v>107.9</v>
       </c>
       <c r="G455" s="4">
         <v>115.4</v>
@@ -23476,7 +23479,7 @@
         <v>121.1</v>
       </c>
       <c r="F456" s="4">
-        <v>108.1</v>
+        <v>108</v>
       </c>
       <c r="G456" s="4">
         <v>116.2</v>
@@ -23485,7 +23488,7 @@
         <v>123</v>
       </c>
       <c r="I456" s="4">
-        <v>107.1</v>
+        <v>107</v>
       </c>
       <c r="J456" s="4">
         <v>54.5</v>
@@ -23523,7 +23526,7 @@
         <v>120.4</v>
       </c>
       <c r="F457" s="4">
-        <v>107.8</v>
+        <v>107.7</v>
       </c>
       <c r="G457" s="4">
         <v>116.2</v>
@@ -23532,7 +23535,7 @@
         <v>122.2</v>
       </c>
       <c r="I457" s="4">
-        <v>106.9</v>
+        <v>106.8</v>
       </c>
       <c r="J457" s="4">
         <v>54.5</v>
@@ -23570,7 +23573,7 @@
         <v>122</v>
       </c>
       <c r="F458" s="4">
-        <v>108.5</v>
+        <v>108.4</v>
       </c>
       <c r="G458" s="4">
         <v>117.3</v>
@@ -23579,7 +23582,7 @@
         <v>123.8</v>
       </c>
       <c r="I458" s="4">
-        <v>107.5</v>
+        <v>107.4</v>
       </c>
       <c r="J458" s="4">
         <v>86.4</v>
@@ -23617,7 +23620,7 @@
         <v>121</v>
       </c>
       <c r="F459" s="4">
-        <v>109</v>
+        <v>108.9</v>
       </c>
       <c r="G459" s="4">
         <v>116.9</v>
@@ -23626,7 +23629,7 @@
         <v>122.8</v>
       </c>
       <c r="I459" s="4">
-        <v>108</v>
+        <v>107.9</v>
       </c>
       <c r="J459" s="4">
         <v>63.6</v>
@@ -23664,7 +23667,7 @@
         <v>121.2</v>
       </c>
       <c r="F460" s="4">
-        <v>110</v>
+        <v>109.9</v>
       </c>
       <c r="G460" s="4">
         <v>116.7</v>
@@ -23673,7 +23676,7 @@
         <v>123.1</v>
       </c>
       <c r="I460" s="4">
-        <v>109</v>
+        <v>108.9</v>
       </c>
       <c r="J460" s="4">
         <v>63.6</v>
@@ -23711,7 +23714,7 @@
         <v>122.8</v>
       </c>
       <c r="F461" s="4">
-        <v>110.2</v>
+        <v>110.1</v>
       </c>
       <c r="G461" s="4">
         <v>118.2</v>
@@ -23720,7 +23723,7 @@
         <v>124.6</v>
       </c>
       <c r="I461" s="4">
-        <v>109.2</v>
+        <v>109.1</v>
       </c>
       <c r="J461" s="4">
         <v>68.2</v>
@@ -23805,7 +23808,7 @@
         <v>122.3</v>
       </c>
       <c r="F463" s="4">
-        <v>110.1</v>
+        <v>110</v>
       </c>
       <c r="G463" s="4">
         <v>116.6</v>
@@ -23852,7 +23855,7 @@
         <v>122</v>
       </c>
       <c r="F464" s="4">
-        <v>110.6</v>
+        <v>110.5</v>
       </c>
       <c r="G464" s="4">
         <v>116.7</v>
@@ -23861,7 +23864,7 @@
         <v>124</v>
       </c>
       <c r="I464" s="4">
-        <v>109.4</v>
+        <v>109.3</v>
       </c>
       <c r="J464" s="4">
         <v>36.4</v>
@@ -23899,7 +23902,7 @@
         <v>122.4</v>
       </c>
       <c r="F465" s="4">
-        <v>110.5</v>
+        <v>110.4</v>
       </c>
       <c r="G465" s="4">
         <v>115.7</v>
@@ -23908,7 +23911,7 @@
         <v>124.4</v>
       </c>
       <c r="I465" s="4">
-        <v>109.3</v>
+        <v>109.2</v>
       </c>
       <c r="J465" s="4">
         <v>18.2</v>
@@ -24181,7 +24184,7 @@
         <v>119.8</v>
       </c>
       <c r="F471" s="4">
-        <v>109.9</v>
+        <v>109.8</v>
       </c>
       <c r="G471" s="4">
         <v>114.4</v>
@@ -24416,7 +24419,7 @@
         <v>119.5</v>
       </c>
       <c r="F476" s="4">
-        <v>110.3</v>
+        <v>110.4</v>
       </c>
       <c r="G476" s="4">
         <v>112.6</v>
@@ -24510,7 +24513,7 @@
         <v>118.7</v>
       </c>
       <c r="F478" s="4">
-        <v>110.1</v>
+        <v>110.2</v>
       </c>
       <c r="G478" s="4">
         <v>111.2</v>
@@ -24886,7 +24889,7 @@
         <v>111.5</v>
       </c>
       <c r="F486" s="4">
-        <v>108.2</v>
+        <v>108.3</v>
       </c>
       <c r="G486" s="4">
         <v>107.3</v>
@@ -24933,7 +24936,7 @@
         <v>110.4</v>
       </c>
       <c r="F487" s="4">
-        <v>107.5</v>
+        <v>107.6</v>
       </c>
       <c r="G487" s="4">
         <v>104.9</v>
@@ -24942,7 +24945,7 @@
         <v>112.5</v>
       </c>
       <c r="I487" s="4">
-        <v>106.6</v>
+        <v>106.7</v>
       </c>
       <c r="J487" s="4">
         <v>36.4</v>
@@ -24989,7 +24992,7 @@
         <v>110.9</v>
       </c>
       <c r="I488" s="4">
-        <v>106.2</v>
+        <v>106.3</v>
       </c>
       <c r="J488" s="4">
         <v>54.5</v>
@@ -25036,7 +25039,7 @@
         <v>108.1</v>
       </c>
       <c r="I489" s="4">
-        <v>105.3</v>
+        <v>105.4</v>
       </c>
       <c r="J489" s="4">
         <v>18.2</v>
@@ -25130,7 +25133,7 @@
         <v>87.2</v>
       </c>
       <c r="I491" s="4">
-        <v>97.2</v>
+        <v>97.1</v>
       </c>
       <c r="J491" s="4">
         <v>9.1</v>
@@ -25168,7 +25171,7 @@
         <v>89.9</v>
       </c>
       <c r="F492" s="4">
-        <v>97.8</v>
+        <v>97.7</v>
       </c>
       <c r="G492" s="4">
         <v>92.3</v>
@@ -25506,7 +25509,7 @@
         <v>107.2</v>
       </c>
       <c r="I499" s="4">
-        <v>97.4</v>
+        <v>97.5</v>
       </c>
       <c r="J499" s="4">
         <v>90.9</v>
@@ -25591,7 +25594,7 @@
         <v>108.9</v>
       </c>
       <c r="F501" s="4">
-        <v>99.3</v>
+        <v>99.4</v>
       </c>
       <c r="G501" s="4">
         <v>115.4</v>
@@ -25694,7 +25697,7 @@
         <v>109.9</v>
       </c>
       <c r="I503" s="4">
-        <v>99.8</v>
+        <v>99.9</v>
       </c>
       <c r="J503" s="4">
         <v>72.7</v>
@@ -25741,7 +25744,7 @@
         <v>110.3</v>
       </c>
       <c r="I504" s="4">
-        <v>100.1</v>
+        <v>100.2</v>
       </c>
       <c r="J504" s="4">
         <v>72.7</v>
@@ -26155,7 +26158,7 @@
         <v>112.1</v>
       </c>
       <c r="F513" s="4">
-        <v>100.5</v>
+        <v>100.6</v>
       </c>
       <c r="G513" s="4">
         <v>112.9</v>
@@ -26249,7 +26252,7 @@
         <v>111.6</v>
       </c>
       <c r="F515" s="4">
-        <v>101</v>
+        <v>101.1</v>
       </c>
       <c r="G515" s="4">
         <v>112.4</v>
@@ -26258,7 +26261,7 @@
         <v>109.7</v>
       </c>
       <c r="I515" s="4">
-        <v>100.8</v>
+        <v>100.9</v>
       </c>
       <c r="J515" s="4">
         <v>36.4</v>
@@ -26296,7 +26299,7 @@
         <v>113.3</v>
       </c>
       <c r="F516" s="4">
-        <v>102.3</v>
+        <v>102.4</v>
       </c>
       <c r="G516" s="4">
         <v>112.4</v>
@@ -26305,7 +26308,7 @@
         <v>112</v>
       </c>
       <c r="I516" s="4">
-        <v>102</v>
+        <v>102.1</v>
       </c>
       <c r="J516" s="4">
         <v>45.5</v>
@@ -26343,7 +26346,7 @@
         <v>113.8</v>
       </c>
       <c r="F517" s="4">
-        <v>102.4</v>
+        <v>102.5</v>
       </c>
       <c r="G517" s="4">
         <v>111.6</v>
@@ -26352,7 +26355,7 @@
         <v>112.5</v>
       </c>
       <c r="I517" s="4">
-        <v>102.1</v>
+        <v>102.2</v>
       </c>
       <c r="J517" s="4">
         <v>31.8</v>
@@ -26390,7 +26393,7 @@
         <v>115</v>
       </c>
       <c r="F518" s="4">
-        <v>103.6</v>
+        <v>103.7</v>
       </c>
       <c r="G518" s="4">
         <v>113.2</v>
@@ -26437,7 +26440,7 @@
         <v>114.5</v>
       </c>
       <c r="F519" s="4">
-        <v>104</v>
+        <v>104.1</v>
       </c>
       <c r="G519" s="4">
         <v>110.8</v>
@@ -26531,7 +26534,7 @@
         <v>113.9</v>
       </c>
       <c r="F521" s="4">
-        <v>104.6</v>
+        <v>104.7</v>
       </c>
       <c r="G521" s="4">
         <v>110.4</v>
@@ -26578,7 +26581,7 @@
         <v>113.3</v>
       </c>
       <c r="F522" s="4">
-        <v>104.3</v>
+        <v>104.4</v>
       </c>
       <c r="G522" s="4">
         <v>109.4</v>
@@ -26587,7 +26590,7 @@
         <v>112.1</v>
       </c>
       <c r="I522" s="4">
-        <v>103.9</v>
+        <v>104</v>
       </c>
       <c r="J522" s="4">
         <v>45.5</v>
@@ -26625,7 +26628,7 @@
         <v>112.9</v>
       </c>
       <c r="F523" s="4">
-        <v>105.8</v>
+        <v>105.9</v>
       </c>
       <c r="G523" s="4">
         <v>108.6</v>
@@ -26634,7 +26637,7 @@
         <v>111.2</v>
       </c>
       <c r="I523" s="4">
-        <v>105.6</v>
+        <v>105.7</v>
       </c>
       <c r="J523" s="4">
         <v>45.5</v>
@@ -26672,7 +26675,7 @@
         <v>114.6</v>
       </c>
       <c r="F524" s="4">
-        <v>105.6</v>
+        <v>105.7</v>
       </c>
       <c r="G524" s="4">
         <v>109.1</v>
@@ -26681,7 +26684,7 @@
         <v>112.9</v>
       </c>
       <c r="I524" s="4">
-        <v>104.7</v>
+        <v>104.8</v>
       </c>
       <c r="J524" s="4">
         <v>54.5</v>
@@ -26719,7 +26722,7 @@
         <v>114.7</v>
       </c>
       <c r="F525" s="4">
-        <v>105.7</v>
+        <v>105.8</v>
       </c>
       <c r="G525" s="4">
         <v>109.2</v>
@@ -26728,7 +26731,7 @@
         <v>113</v>
       </c>
       <c r="I525" s="4">
-        <v>104.7</v>
+        <v>104.8</v>
       </c>
       <c r="J525" s="4">
         <v>54.5</v>
@@ -26766,7 +26769,7 @@
         <v>114.7</v>
       </c>
       <c r="F526" s="4">
-        <v>106</v>
+        <v>106.1</v>
       </c>
       <c r="G526" s="4">
         <v>109</v>
@@ -26822,7 +26825,7 @@
         <v>113.7</v>
       </c>
       <c r="I527" s="4">
-        <v>105.5</v>
+        <v>105.6</v>
       </c>
       <c r="J527" s="4">
         <v>40.9</v>
@@ -26869,7 +26872,7 @@
         <v>113.6</v>
       </c>
       <c r="I528" s="4">
-        <v>105.6</v>
+        <v>105.7</v>
       </c>
       <c r="J528" s="4">
         <v>72.7</v>
@@ -27057,7 +27060,7 @@
         <v>113.9</v>
       </c>
       <c r="I532" s="4">
-        <v>106.1</v>
+        <v>106</v>
       </c>
       <c r="J532" s="4">
         <v>27.3</v>
@@ -27151,7 +27154,7 @@
         <v>114.3</v>
       </c>
       <c r="I534" s="4">
-        <v>106.7</v>
+        <v>106.6</v>
       </c>
       <c r="J534" s="4">
         <v>45.5</v>
@@ -27198,7 +27201,7 @@
         <v>111</v>
       </c>
       <c r="I535" s="4">
-        <v>105</v>
+        <v>104.9</v>
       </c>
       <c r="J535" s="4">
         <v>54.5</v>
@@ -27471,7 +27474,7 @@
         <v>115.6</v>
       </c>
       <c r="F541" s="4">
-        <v>108.7</v>
+        <v>108.8</v>
       </c>
       <c r="G541" s="4">
         <v>109.8</v>
@@ -27715,7 +27718,7 @@
         <v>114.4</v>
       </c>
       <c r="I546" s="4">
-        <v>108</v>
+        <v>108.1</v>
       </c>
       <c r="J546" s="4">
         <v>45.5</v>
@@ -27753,7 +27756,7 @@
         <v>116.3</v>
       </c>
       <c r="F547" s="4">
-        <v>111.5</v>
+        <v>111.6</v>
       </c>
       <c r="G547" s="4">
         <v>109.1</v>
@@ -28035,7 +28038,7 @@
         <v>114.3</v>
       </c>
       <c r="F553" s="4">
-        <v>113.6</v>
+        <v>113.5</v>
       </c>
       <c r="G553" s="4">
         <v>106.1</v>
@@ -28091,7 +28094,7 @@
         <v>111.7</v>
       </c>
       <c r="I554" s="4">
-        <v>110.2</v>
+        <v>110.1</v>
       </c>
       <c r="J554" s="4">
         <v>54.5</v>
@@ -28170,40 +28173,40 @@
         <v>10</v>
       </c>
       <c r="D556" s="4">
+        <v>109.8</v>
+      </c>
+      <c r="E556" s="4">
+        <v>115.9</v>
+      </c>
+      <c r="F556" s="4">
+        <v>112.2</v>
+      </c>
+      <c r="G556" s="4">
+        <v>109.7</v>
+      </c>
+      <c r="H556" s="4">
+        <v>114.3</v>
+      </c>
+      <c r="I556" s="4">
         <v>110</v>
       </c>
-      <c r="E556" s="4">
-        <v>115.4</v>
-      </c>
-      <c r="F556" s="4">
-        <v>112.6</v>
-      </c>
-      <c r="G556" s="4">
-        <v>110</v>
-      </c>
-      <c r="H556" s="4">
-        <v>113.8</v>
-      </c>
-      <c r="I556" s="4">
-        <v>110.4</v>
-      </c>
       <c r="J556" s="4">
-        <v>88.9</v>
+        <v>90</v>
       </c>
       <c r="K556" s="4">
-        <v>75</v>
+        <v>66.7</v>
       </c>
       <c r="L556" s="4">
-        <v>25</v>
+        <v>37.5</v>
       </c>
       <c r="M556" s="4">
-        <v>1256</v>
+        <v>1257.0999999999999</v>
       </c>
       <c r="N556" s="4">
-        <v>3220</v>
+        <v>3211.7</v>
       </c>
       <c r="O556" s="4">
-        <v>3215.8</v>
+        <v>3228.3</v>
       </c>
     </row>
     <row r="565" spans="4:9" x14ac:dyDescent="0.2">

</xml_diff>